<commit_message>
Corrección ejercicio busqueda tema 3
</commit_message>
<xml_diff>
--- a/03_OSINT/Máster Ciberseguridad - M3 - OSINT - Operadores avanzados de búsqueda.xlsx
+++ b/03_OSINT/Máster Ciberseguridad - M3 - OSINT - Operadores avanzados de búsqueda.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Tech\ENIIT\Ciberseguridad\03_OSINT\01_Tarea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Tech\ENIIT\MasterCiberseguridad\03_OSINT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E2717C-A94F-4F59-8BE4-D382F1F8C4C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4050F6-BD81-4683-A111-88D969DAF953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operadores_búsqueda" sheetId="2" r:id="rId1"/>
+    <sheet name="Ejemplos_Avanzados" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>FUNCIONALIDAD</t>
   </si>
@@ -215,13 +216,64 @@
   </si>
   <si>
     <t>ip</t>
+  </si>
+  <si>
+    <t>¿Cuál sería la expresión correspondiente a la búsqueda de ficheros xls que contengan las palabras user y password dentro de un servidor ftp?</t>
+  </si>
+  <si>
+    <t>ext:xls inurl:"ftp://" user password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cómo identificarías páginas gubernamentales que han sido hackeadas? La frase exacta debe ser:"hacked by". </t>
+  </si>
+  <si>
+    <t>site:gob.* "hacked by"</t>
+  </si>
+  <si>
+    <t>¿Cómo identificarías algún sistema SCADA?</t>
+  </si>
+  <si>
+    <t>¿Cómo identificarías en sitios gubernamentales algún fichero ofimático con la marca de confidencial?</t>
+  </si>
+  <si>
+    <t>¿Podrías identificar algún tipo de vulnerabilidad en alguna página gubernamental peruana?</t>
+  </si>
+  <si>
+    <t>inurl:"Portal/Portal.mwsl"</t>
+  </si>
+  <si>
+    <t>https://www.flu-project.com/2016/05/google-hacking-de-sistemas-scada-de.html</t>
+  </si>
+  <si>
+    <t>https://www.hackers-arise.com/post/2016/07/05/scada-hacking-finding-vulnerable-scada-systems-using-google-hacking</t>
+  </si>
+  <si>
+    <t>allintitle:confidential filetype:doc site:gob</t>
+  </si>
+  <si>
+    <t>“robots.txt” “disallow:” filetype:txt site:gob</t>
+  </si>
+  <si>
+    <t>Usando los ejemplos anteriores:</t>
+  </si>
+  <si>
+    <t>“robots.txt” “disallow:” filetype:txt site:gob.pe</t>
+  </si>
+  <si>
+    <t>Se pueden ficheros que no quieren que sean indexados.</t>
+  </si>
+  <si>
+    <t>allintitle:confidential filetype:pdf site:gob.pe</t>
+  </si>
+  <si>
+    <t>Algunos documentos confidenciales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -259,6 +311,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF373B41"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -287,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +356,14 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -581,11 +647,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -934,4 +1000,114 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44B41C8-2429-4C54-A54F-007346167B74}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="80.85546875" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="I3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>